<commit_message>
New future enhancement added
</commit_message>
<xml_diff>
--- a/AutoTourism To Do.xlsx
+++ b/AutoTourism To Do.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>No</t>
   </si>
@@ -52,14 +52,40 @@
   </si>
   <si>
     <t>Personalization of folder (Sort, View)</t>
+  </si>
+  <si>
+    <t>Multiple Payment for one invoice</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Revert check out in case of operator mistake</t>
+  </si>
+  <si>
+    <t>Checkin</t>
+  </si>
+  <si>
+    <t>Recycle bin</t>
+  </si>
+  <si>
+    <t>Navigator and all component</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,37 +417,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="71.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -478,9 +505,47 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
New point for automatic report added
</commit_message>
<xml_diff>
--- a/AutoTourism To Do.xlsx
+++ b/AutoTourism To Do.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>No</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Navigator and all component</t>
+  </si>
+  <si>
+    <t>Automatic report generation</t>
+  </si>
+  <si>
+    <t>Report</t>
   </si>
 </sst>
 </file>
@@ -417,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,6 +549,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>